<commit_message>
Further attempt to create function check button in Farm tab (unsuccessful).
</commit_message>
<xml_diff>
--- a/OratorRun/study_areas/Dummy (IND)/Grassland/FarmWthrMgmt.xlsx
+++ b/OratorRun/study_areas/Dummy (IND)/Grassland/FarmWthrMgmt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pyorator\study_areas\Dummy (IND)\Grassland\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\testPyOra\OratorRun\study_areas\Dummy (IND)\Grassland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E14A640-D689-438F-80C9-112A6BAA3572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{088A0B7E-79C6-497C-B000-93390241E82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4035" yWindow="2880" windowWidth="18780" windowHeight="12735" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1065" yWindow="2790" windowWidth="25785" windowHeight="14685" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Signature" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="80">
   <si>
     <t>Attribute</t>
   </si>
@@ -727,7 +727,7 @@
   <dimension ref="A1:J361"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B104" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B330" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
@@ -7261,13 +7261,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F361"/>
+  <dimension ref="A1:F360"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B222" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B329" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H236" sqref="H236"/>
+      <selection pane="bottomRight" activeCell="I335" sqref="I335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14473,26 +14473,6 @@
         <v>25.9</v>
       </c>
       <c r="F360" s="4">
-        <v>1931</v>
-      </c>
-    </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A361" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B361" s="4">
-        <v>9</v>
-      </c>
-      <c r="C361">
-        <v>12</v>
-      </c>
-      <c r="D361">
-        <v>3.6</v>
-      </c>
-      <c r="E361">
-        <v>25.9</v>
-      </c>
-      <c r="F361" s="4">
         <v>1931</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add hwsd files .hdr and .bil
</commit_message>
<xml_diff>
--- a/OratorRun/study_areas/Dummy (IND)/Grassland/FarmWthrMgmt.xlsx
+++ b/OratorRun/study_areas/Dummy (IND)/Grassland/FarmWthrMgmt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\testPyOra\OratorRun\study_areas\Dummy (IND)\Grassland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{088A0B7E-79C6-497C-B000-93390241E82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDB1FF4-828E-476D-B4FB-E25947C8B302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="2790" windowWidth="25785" windowHeight="14685" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1365" yWindow="1560" windowWidth="27435" windowHeight="14685" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Signature" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="80">
   <si>
     <t>Attribute</t>
   </si>
@@ -7261,13 +7261,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F360"/>
+  <dimension ref="A1:F361"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B329" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B338" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I335" sqref="I335"/>
+      <selection pane="bottomRight" activeCell="M348" sqref="M348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14473,6 +14473,26 @@
         <v>25.9</v>
       </c>
       <c r="F360" s="4">
+        <v>1931</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A361" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B361" s="4">
+        <v>9</v>
+      </c>
+      <c r="C361">
+        <v>12</v>
+      </c>
+      <c r="D361">
+        <v>3.6</v>
+      </c>
+      <c r="E361">
+        <v>25.9</v>
+      </c>
+      <c r="F361" s="4">
         <v>1931</v>
       </c>
     </row>

</xml_diff>